<commit_message>
add gmail automation sending
</commit_message>
<xml_diff>
--- a/assets/form_penilaian_alkes.xlsx
+++ b/assets/form_penilaian_alkes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\githubdownload\flutter_application_1\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63391E18-3486-47B4-969A-957A7712348A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AD340C-B29D-4AF1-ACF4-854A9F8C0417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0EB2990C-F5BD-4C81-A27D-33F34D5291FD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
   <si>
     <t>Set Pemeriksaan Umum</t>
   </si>
@@ -217,12 +217,27 @@
 Minimum Alat 
 Kesehatan : 60</t>
   </si>
+  <si>
+    <t>Header1</t>
+  </si>
+  <si>
+    <t>Nama Indikator</t>
+  </si>
+  <si>
+    <t>Sub Indikator</t>
+  </si>
+  <si>
+    <t>Pertanyaan</t>
+  </si>
+  <si>
+    <t>Kriteria</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +253,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -247,7 +269,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -255,11 +277,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -268,6 +305,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,19 +640,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57D4D6C-AE1B-4EE5-82FF-B7B83771CABB}">
-  <dimension ref="A2:C24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
-    <col min="3" max="5" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -624,8 +681,14 @@
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -635,8 +698,14 @@
       <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -646,8 +715,14 @@
       <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -657,8 +732,14 @@
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -668,8 +749,14 @@
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -679,8 +766,14 @@
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -690,8 +783,14 @@
       <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -701,8 +800,14 @@
       <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -712,8 +817,14 @@
       <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -723,8 +834,14 @@
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -734,8 +851,14 @@
       <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -745,8 +868,14 @@
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -756,8 +885,14 @@
       <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -767,8 +902,14 @@
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -778,8 +919,14 @@
       <c r="C16" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -789,8 +936,14 @@
       <c r="C17" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -800,8 +953,14 @@
       <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -811,8 +970,14 @@
       <c r="C19" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -822,8 +987,14 @@
       <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -833,8 +1004,14 @@
       <c r="C21" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -844,8 +1021,14 @@
       <c r="C22" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -855,8 +1038,14 @@
       <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -865,6 +1054,12 @@
       </c>
       <c r="C24" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function penilaiam alkess
</commit_message>
<xml_diff>
--- a/assets/form_penilaian_alkes.xlsx
+++ b/assets/form_penilaian_alkes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\githubdownload\flutter_application_1\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AD340C-B29D-4AF1-ACF4-854A9F8C0417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9F744F-730B-428C-B3B9-F64E6BE276C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0EB2990C-F5BD-4C81-A27D-33F34D5291FD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t>Set Pemeriksaan Umum</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Kriteria</t>
+  </si>
+  <si>
+    <t>anjay</t>
   </si>
 </sst>
 </file>
@@ -642,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57D4D6C-AE1B-4EE5-82FF-B7B83771CABB}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +674,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -685,7 +688,7 @@
         <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
YALLAH SEMOGA INI TERAKHIR YAA, ALHAMDULILLAH YA ALLAH PLISssss
</commit_message>
<xml_diff>
--- a/assets/form_penilaian_alkes.xlsx
+++ b/assets/form_penilaian_alkes.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\githubdownload\flutter_application_1\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE85B08-A721-4EAA-A0EC-48661CF13BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>Header1</t>
   </si>
@@ -51,32 +57,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Jumlah 
-Minimum Alat 
-Kesehatan : </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>28</t>
-    </r>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t xml:space="preserve">Set Tindakan Medis/Gawat Darurat </t>
-  </si>
-  <si>
-    <t>Jumlah 
-Minimum Alat 
-Kesehatan : 125</t>
   </si>
   <si>
     <t>Jumlah 
@@ -248,11 +232,6 @@
   </si>
   <si>
     <t xml:space="preserve">Set Rawat Inap </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumlah 
-Minimum Alat 
-Kesehatan :  124-132 </t>
   </si>
   <si>
     <t xml:space="preserve">Jumlah 
@@ -354,12 +333,22 @@
   <si>
     <t xml:space="preserve">Kit Kesehatan Lingkungan </t>
   </si>
+  <si>
+    <t>x Indikator 1: Kelengkapan alat kesehatan (lihat di lampiran: jumlah minimum alat
+kesehatan)
+d) Jika set alat kesehatan lengkap, maka nilai 2
+e) Jika set alat kesehatan tidak lengkap, maka nilai 1
+f) Jika tidak ada set alat kesehatan, maka nilai 0
+x Indikator 2: Uji alat/kalibrasi alat kesehatan
+d) Jika set alat kesehatan rutin diuji/kalibrasi, maka nilai 2
+e) Jika set alat kesehatan pernah diuji namun tidak rutin, maka nilai 1
+f) Jika tidak pernah menguji/mengkalibrasi alat kesehatan, maka nilai 0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,58 +426,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -499,10 +489,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -540,71 +530,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -632,7 +622,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -655,11 +645,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -668,13 +658,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -684,7 +674,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -693,7 +683,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -702,7 +692,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -710,10 +700,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -778,24 +768,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="44.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,7 +804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="51.75">
+    <row r="2" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -822,385 +814,385 @@
       <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
+      <c r="D2" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
+      <c r="D3" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="51.75">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="51.75">
+    </row>
+    <row r="12" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="64.5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="51.75">
+    </row>
+    <row r="15" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="51.75">
+    </row>
+    <row r="18" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="51.75">
+    </row>
+    <row r="19" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="51.75">
+    </row>
+    <row r="22" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="51.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>